<commit_message>
update site 47 spreadsheet SEDBIOME
</commit_message>
<xml_diff>
--- a/assets/projects/sed-biome/data-entry-spreadsheets/SED-BIOME_site-47_Panama.xlsx
+++ b/assets/projects/sed-biome/data-entry-spreadsheets/SED-BIOME_site-47_Panama.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lonnemanm\Documents\repositories\marinegeo.github.io\assets\projects\sed-biome\data-entry-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEAEF87-D62E-4074-A38D-202FF991DFBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EEE7F6-E949-4DEE-A80E-89177B82913D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="1125" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="316">
   <si>
     <t>sheet</t>
   </si>
@@ -546,82 +546,67 @@
     <t>sediment sample - organic matter</t>
   </si>
   <si>
+    <t>Site 47 - C - B1</t>
+  </si>
+  <si>
     <t>36.2984</t>
   </si>
   <si>
+    <t>Site 47 - C - B2</t>
+  </si>
+  <si>
+    <t>Site 47 - C - B3</t>
+  </si>
+  <si>
+    <t>Site 47 - F - B1</t>
+  </si>
+  <si>
+    <t>Site 47 - F - B2</t>
+  </si>
+  <si>
+    <t>Site 47 - F - B3</t>
+  </si>
+  <si>
     <t>control</t>
   </si>
   <si>
+    <t>Site 47 - C1</t>
+  </si>
+  <si>
     <t>rooibos</t>
-  </si>
-  <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>fertilised</t>
-  </si>
-  <si>
-    <t>Panama</t>
-  </si>
-  <si>
-    <t>Naos laboratories</t>
-  </si>
-  <si>
-    <t>Site47-C-Sediment #1</t>
-  </si>
-  <si>
-    <t>Site47-C-Sediment #2</t>
-  </si>
-  <si>
-    <t>Site47-F-Sediment #1</t>
-  </si>
-  <si>
-    <t>Site47-F-Sediment #2</t>
-  </si>
-  <si>
-    <t>Site47-C1</t>
-  </si>
-  <si>
-    <t>Site47-C2</t>
-  </si>
-  <si>
-    <t>Site47-C3</t>
-  </si>
-  <si>
-    <t>Site47-C4</t>
-  </si>
-  <si>
-    <t>Site47-F1</t>
-  </si>
-  <si>
-    <t>Site47-F2</t>
-  </si>
-  <si>
-    <t>Site47-F3</t>
-  </si>
-  <si>
-    <t>Site47-F4</t>
-  </si>
-  <si>
-    <t>Site 47 - C1</t>
   </si>
   <si>
     <t>Site 47 - C1
  Rooibos 1</t>
   </si>
   <si>
+    <t>S47-R1</t>
+  </si>
+  <si>
     <t>Site 47 - C1
  Rooibos 2</t>
   </si>
   <si>
+    <t>S47-R2</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
     <t>Site 47 - C1
  Green 1</t>
   </si>
   <si>
+    <t>S47-G1</t>
+  </si>
+  <si>
     <t>Site 47 - C1
  Green 2</t>
   </si>
   <si>
+    <t>S47-G2</t>
+  </si>
+  <si>
     <t>Site 47 - C2</t>
   </si>
   <si>
@@ -629,18 +614,30 @@
  Rooibos 3</t>
   </si>
   <si>
+    <t>S47-R3</t>
+  </si>
+  <si>
     <t>Site 47 - C2
  Rooibos 4</t>
   </si>
   <si>
+    <t>S47-R4</t>
+  </si>
+  <si>
     <t>Site 47 - C2
  Green 3</t>
   </si>
   <si>
+    <t>S47-G3</t>
+  </si>
+  <si>
     <t>Site 47 - C2
  Green 4</t>
   </si>
   <si>
+    <t>S47-G4</t>
+  </si>
+  <si>
     <t>Site 47 - C3</t>
   </si>
   <si>
@@ -648,18 +645,30 @@
  Rooibos 5</t>
   </si>
   <si>
+    <t>S47-R5</t>
+  </si>
+  <si>
     <t>Site 47 - C3
  Rooibos 6</t>
   </si>
   <si>
+    <t>S47-R6</t>
+  </si>
+  <si>
     <t>Site 47 - C3
  Green 5</t>
   </si>
   <si>
+    <t>S47-G5</t>
+  </si>
+  <si>
     <t>Site 47 - C3
  Green 6</t>
   </si>
   <si>
+    <t>S47-G6</t>
+  </si>
+  <si>
     <t>Site 47 - C4</t>
   </si>
   <si>
@@ -667,18 +676,30 @@
  Rooibos 7</t>
   </si>
   <si>
+    <t>S47-R7</t>
+  </si>
+  <si>
     <t>Site 47 - C4
  Rooibos 8</t>
   </si>
   <si>
+    <t>S47-R8</t>
+  </si>
+  <si>
     <t>Site 47 - C4
  Green 7</t>
   </si>
   <si>
+    <t>S47-G7</t>
+  </si>
+  <si>
     <t>Site 47 - C4
  Green 8</t>
   </si>
   <si>
+    <t>S47-G8</t>
+  </si>
+  <si>
     <t>Site 47 - C5</t>
   </si>
   <si>
@@ -686,18 +707,30 @@
  Rooibos 9</t>
   </si>
   <si>
+    <t>S47-R9</t>
+  </si>
+  <si>
     <t>Site 47 - C5
  Rooibos 10</t>
   </si>
   <si>
+    <t>S47-R10</t>
+  </si>
+  <si>
     <t>Site 47 - C5
  Green 9</t>
   </si>
   <si>
+    <t>S47-G9</t>
+  </si>
+  <si>
     <t>Site 47 - C5
  Green 10</t>
   </si>
   <si>
+    <t>S47-G10</t>
+  </si>
+  <si>
     <t>Site 47 - C6</t>
   </si>
   <si>
@@ -705,18 +738,30 @@
  Rooibos 11</t>
   </si>
   <si>
+    <t>S47-R11</t>
+  </si>
+  <si>
     <t>Site 47 - C6
  Rooibos 12</t>
   </si>
   <si>
+    <t>S47-R12</t>
+  </si>
+  <si>
     <t>Site 47 - C6
  Green 11</t>
   </si>
   <si>
+    <t>S47-G11</t>
+  </si>
+  <si>
     <t>Site 47 - C6
  Green 12</t>
   </si>
   <si>
+    <t>S47-G12</t>
+  </si>
+  <si>
     <t>Site 47 - C7</t>
   </si>
   <si>
@@ -724,18 +769,30 @@
  Rooibos 13</t>
   </si>
   <si>
+    <t>S47-R13</t>
+  </si>
+  <si>
     <t>Site 47 - C7
  Rooibos 14</t>
   </si>
   <si>
+    <t>S47-R14</t>
+  </si>
+  <si>
     <t>Site 47 - C7
  Green 13</t>
   </si>
   <si>
+    <t>S47-G13</t>
+  </si>
+  <si>
     <t>Site 47 - C7
  Green 14</t>
   </si>
   <si>
+    <t>S47-G14</t>
+  </si>
+  <si>
     <t>Site 47 - C8</t>
   </si>
   <si>
@@ -743,18 +800,33 @@
  Rooibos 15</t>
   </si>
   <si>
+    <t>S47-R15</t>
+  </si>
+  <si>
     <t>Site 47 - C8
  Rooibos 16</t>
   </si>
   <si>
+    <t>S47-R16</t>
+  </si>
+  <si>
     <t>Site 47 - C8
  Green 15</t>
   </si>
   <si>
+    <t>S47-G15</t>
+  </si>
+  <si>
     <t>Site 47 - C8
  Green 16</t>
   </si>
   <si>
+    <t>S47-G16</t>
+  </si>
+  <si>
+    <t>fertilised</t>
+  </si>
+  <si>
     <t>Site 47 - F1</t>
   </si>
   <si>
@@ -762,18 +834,30 @@
  Rooibos 17</t>
   </si>
   <si>
+    <t>S47-R17</t>
+  </si>
+  <si>
     <t>Site 47 - F1
  Rooibos 18</t>
   </si>
   <si>
+    <t>S47-R18</t>
+  </si>
+  <si>
     <t>Site 47 - F1
  Green 17</t>
   </si>
   <si>
+    <t>S47-G17</t>
+  </si>
+  <si>
     <t>Site 47 - F1
  Green 18</t>
   </si>
   <si>
+    <t>S47-G18</t>
+  </si>
+  <si>
     <t>Site 47 - F2</t>
   </si>
   <si>
@@ -781,18 +865,30 @@
  Rooibos 19</t>
   </si>
   <si>
+    <t>S47-R19</t>
+  </si>
+  <si>
     <t>Site 47 - F2
  Rooibos 20</t>
   </si>
   <si>
+    <t>S47-R20</t>
+  </si>
+  <si>
     <t>Site 47 - F2
  Green 19</t>
   </si>
   <si>
+    <t>S47-G19</t>
+  </si>
+  <si>
     <t>Site 47 - F2
  Green 20</t>
   </si>
   <si>
+    <t>S47-G20</t>
+  </si>
+  <si>
     <t>Site 47 - F3</t>
   </si>
   <si>
@@ -800,18 +896,30 @@
  Rooibos 21</t>
   </si>
   <si>
+    <t>S47-R21</t>
+  </si>
+  <si>
     <t>Site 47 - F3
  Rooibos 22</t>
   </si>
   <si>
+    <t>S47-R22</t>
+  </si>
+  <si>
     <t>Site 47 - F3
  Green 21</t>
   </si>
   <si>
+    <t>S47-G21</t>
+  </si>
+  <si>
     <t>Site 47 - F3
  Green 22</t>
   </si>
   <si>
+    <t>S47-G22</t>
+  </si>
+  <si>
     <t>Site 47 - F4</t>
   </si>
   <si>
@@ -819,18 +927,30 @@
  Rooibos 23</t>
   </si>
   <si>
+    <t>S47-R23</t>
+  </si>
+  <si>
     <t>Site 47 - F4
  Rooibos 24</t>
   </si>
   <si>
+    <t>S47-R24</t>
+  </si>
+  <si>
     <t>Site 47 - F4
  Green 23</t>
   </si>
   <si>
+    <t>S47-G23</t>
+  </si>
+  <si>
     <t>Site 47 - F4
  Green 24</t>
   </si>
   <si>
+    <t>S47-G24</t>
+  </si>
+  <si>
     <t>Site 47 - F5</t>
   </si>
   <si>
@@ -838,18 +958,30 @@
  Rooibos 25</t>
   </si>
   <si>
+    <t>S47-R25</t>
+  </si>
+  <si>
     <t>Site 47 - F5
  Rooibos 26</t>
   </si>
   <si>
+    <t>S47-R26</t>
+  </si>
+  <si>
     <t>Site 47 - F5
  Green 25</t>
   </si>
   <si>
+    <t>S47-G25</t>
+  </si>
+  <si>
     <t>Site 47 - F5
  Green 26</t>
   </si>
   <si>
+    <t>S47-G26</t>
+  </si>
+  <si>
     <t>Site 47 - F6</t>
   </si>
   <si>
@@ -857,18 +989,30 @@
  Rooibos 27</t>
   </si>
   <si>
+    <t>S47-R27</t>
+  </si>
+  <si>
     <t>Site 47 - F6
  Rooibos 28</t>
   </si>
   <si>
+    <t>S47-R28</t>
+  </si>
+  <si>
     <t>Site 47 - F6
  Green 27</t>
   </si>
   <si>
+    <t>S47-G27</t>
+  </si>
+  <si>
     <t>Site 47 - F6
  Green 28</t>
   </si>
   <si>
+    <t>S47-G28</t>
+  </si>
+  <si>
     <t>Site 47 - F7</t>
   </si>
   <si>
@@ -876,18 +1020,30 @@
  Rooibos 29</t>
   </si>
   <si>
+    <t>S47-R29</t>
+  </si>
+  <si>
     <t>Site 47 - F7
  Rooibos 30</t>
   </si>
   <si>
+    <t>S47-R30</t>
+  </si>
+  <si>
     <t>Site 47 - F7
  Green 29</t>
   </si>
   <si>
+    <t>S47-G29</t>
+  </si>
+  <si>
     <t>Site 47 - F7
  Green 30</t>
   </si>
   <si>
+    <t>S47-G30</t>
+  </si>
+  <si>
     <t>Site 47 - F8</t>
   </si>
   <si>
@@ -895,226 +1051,67 @@
  Rooibos 31</t>
   </si>
   <si>
+    <t>S47-R31</t>
+  </si>
+  <si>
     <t>Site 47 - F8
  Rooibos 32</t>
   </si>
   <si>
+    <t>S47-R32</t>
+  </si>
+  <si>
     <t>Site 47 - F8
  Green 31</t>
   </si>
   <si>
+    <t>S47-G31</t>
+  </si>
+  <si>
     <t>Site 47 - F8
  Green 32</t>
   </si>
   <si>
-    <t>Site 47 - C - B1</t>
-  </si>
-  <si>
-    <t>Site 47 - C - B2</t>
-  </si>
-  <si>
-    <t>Site 47 - C - B3</t>
-  </si>
-  <si>
-    <t>Site 47 - F - B1</t>
-  </si>
-  <si>
-    <t>Site 47 - F - B2</t>
-  </si>
-  <si>
-    <t>Site 47 - F - B3</t>
-  </si>
-  <si>
-    <t>S47-R1</t>
-  </si>
-  <si>
-    <t>S47-R2</t>
-  </si>
-  <si>
-    <t>S47-G1</t>
-  </si>
-  <si>
-    <t>S47-G2</t>
-  </si>
-  <si>
-    <t>S47-R3</t>
-  </si>
-  <si>
-    <t>S47-R4</t>
-  </si>
-  <si>
-    <t>S47-G3</t>
-  </si>
-  <si>
-    <t>S47-G4</t>
-  </si>
-  <si>
-    <t>S47-R5</t>
-  </si>
-  <si>
-    <t>S47-R6</t>
-  </si>
-  <si>
-    <t>S47-G5</t>
-  </si>
-  <si>
-    <t>S47-G6</t>
-  </si>
-  <si>
-    <t>S47-R7</t>
-  </si>
-  <si>
-    <t>S47-R8</t>
-  </si>
-  <si>
-    <t>S47-G7</t>
-  </si>
-  <si>
-    <t>S47-G8</t>
-  </si>
-  <si>
-    <t>S47-R9</t>
-  </si>
-  <si>
-    <t>S47-R10</t>
-  </si>
-  <si>
-    <t>S47-G9</t>
-  </si>
-  <si>
-    <t>S47-G10</t>
-  </si>
-  <si>
-    <t>S47-R11</t>
-  </si>
-  <si>
-    <t>S47-R12</t>
-  </si>
-  <si>
-    <t>S47-G11</t>
-  </si>
-  <si>
-    <t>S47-G12</t>
-  </si>
-  <si>
-    <t>S47-R13</t>
-  </si>
-  <si>
-    <t>S47-R14</t>
-  </si>
-  <si>
-    <t>S47-G13</t>
-  </si>
-  <si>
-    <t>S47-G14</t>
-  </si>
-  <si>
-    <t>S47-R15</t>
-  </si>
-  <si>
-    <t>S47-R16</t>
-  </si>
-  <si>
-    <t>S47-G15</t>
-  </si>
-  <si>
-    <t>S47-G16</t>
-  </si>
-  <si>
-    <t>S47-R17</t>
-  </si>
-  <si>
-    <t>S47-R18</t>
-  </si>
-  <si>
-    <t>S47-G17</t>
-  </si>
-  <si>
-    <t>S47-G18</t>
-  </si>
-  <si>
-    <t>S47-R19</t>
-  </si>
-  <si>
-    <t>S47-R20</t>
-  </si>
-  <si>
-    <t>S47-G19</t>
-  </si>
-  <si>
-    <t>S47-G20</t>
-  </si>
-  <si>
-    <t>S47-R21</t>
-  </si>
-  <si>
-    <t>S47-R22</t>
-  </si>
-  <si>
-    <t>S47-G21</t>
-  </si>
-  <si>
-    <t>S47-G22</t>
-  </si>
-  <si>
-    <t>S47-R23</t>
-  </si>
-  <si>
-    <t>S47-R24</t>
-  </si>
-  <si>
-    <t>S47-G23</t>
-  </si>
-  <si>
-    <t>S47-G24</t>
-  </si>
-  <si>
-    <t>S47-R25</t>
-  </si>
-  <si>
-    <t>S47-R26</t>
-  </si>
-  <si>
-    <t>S47-G25</t>
-  </si>
-  <si>
-    <t>S47-G26</t>
-  </si>
-  <si>
-    <t>S47-R27</t>
-  </si>
-  <si>
-    <t>S47-R28</t>
-  </si>
-  <si>
-    <t>S47-G27</t>
-  </si>
-  <si>
-    <t>S47-G28</t>
-  </si>
-  <si>
-    <t>S47-R29</t>
-  </si>
-  <si>
-    <t>S47-R30</t>
-  </si>
-  <si>
-    <t>S47-G29</t>
-  </si>
-  <si>
-    <t>S47-G30</t>
-  </si>
-  <si>
-    <t>S47-R31</t>
-  </si>
-  <si>
-    <t>S47-R32</t>
-  </si>
-  <si>
-    <t>S47-G31</t>
-  </si>
-  <si>
     <t>S47-G32</t>
+  </si>
+  <si>
+    <t>Site47-C-Sediment #1</t>
+  </si>
+  <si>
+    <t>Site47-C-Sediment #2</t>
+  </si>
+  <si>
+    <t>Site47-F-Sediment #1</t>
+  </si>
+  <si>
+    <t>Site47-F-Sediment #2</t>
+  </si>
+  <si>
+    <t>Site47-C1</t>
+  </si>
+  <si>
+    <t>Site47-C2</t>
+  </si>
+  <si>
+    <t>Site47-C3</t>
+  </si>
+  <si>
+    <t>Site47-C4</t>
+  </si>
+  <si>
+    <t>Site47-F1</t>
+  </si>
+  <si>
+    <t>Site47-F2</t>
+  </si>
+  <si>
+    <t>Site47-F3</t>
+  </si>
+  <si>
+    <t>Site47-F4</t>
+  </si>
+  <si>
+    <t>Panama</t>
   </si>
 </sst>
 </file>
@@ -1332,7 +1329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1457,10 +1454,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2063,7 +2056,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="39.950000000000003" customHeight="1"/>
@@ -2202,7 +2195,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2276,11 +2269,9 @@
         <v>47</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>154</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="C2" s="11"/>
       <c r="J2" s="11"/>
       <c r="M2" s="2"/>
     </row>
@@ -2603,7 +2594,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2645,7 +2636,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>303</v>
       </c>
       <c r="C2" t="s">
         <v>147</v>
@@ -2656,7 +2647,7 @@
         <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>304</v>
       </c>
       <c r="C3" t="s">
         <v>147</v>
@@ -2667,7 +2658,7 @@
         <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>305</v>
       </c>
       <c r="C4" t="s">
         <v>147</v>
@@ -2678,7 +2669,7 @@
         <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>306</v>
       </c>
       <c r="C5" t="s">
         <v>147</v>
@@ -2689,7 +2680,7 @@
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>307</v>
       </c>
       <c r="C6" t="s">
         <v>130</v>
@@ -2700,7 +2691,7 @@
         <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>308</v>
       </c>
       <c r="C7" t="s">
         <v>130</v>
@@ -2711,7 +2702,7 @@
         <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>309</v>
       </c>
       <c r="C8" t="s">
         <v>130</v>
@@ -2722,7 +2713,7 @@
         <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
+        <v>310</v>
       </c>
       <c r="C9" t="s">
         <v>130</v>
@@ -2733,7 +2724,7 @@
         <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>311</v>
       </c>
       <c r="C10" t="s">
         <v>130</v>
@@ -2744,7 +2735,7 @@
         <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>164</v>
+        <v>312</v>
       </c>
       <c r="C11" t="s">
         <v>130</v>
@@ -2755,7 +2746,7 @@
         <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>165</v>
+        <v>313</v>
       </c>
       <c r="C12" t="s">
         <v>130</v>
@@ -2766,7 +2757,7 @@
         <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
+        <v>314</v>
       </c>
       <c r="C13" t="s">
         <v>130</v>
@@ -2922,22 +2913,22 @@
         <v>47</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H2" s="45" t="s">
-        <v>168</v>
+        <v>157</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="I2" t="s">
-        <v>253</v>
+        <v>159</v>
       </c>
       <c r="J2"/>
     </row>
@@ -2948,22 +2939,22 @@
         <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H3" s="45" t="s">
-        <v>169</v>
+        <v>157</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="I3" t="s">
-        <v>254</v>
+        <v>161</v>
       </c>
       <c r="J3"/>
     </row>
@@ -2974,22 +2965,22 @@
         <v>47</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H4" s="45" t="s">
-        <v>170</v>
+        <v>162</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="I4" t="s">
-        <v>255</v>
+        <v>164</v>
       </c>
       <c r="J4"/>
     </row>
@@ -3000,22 +2991,22 @@
         <v>47</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H5" s="45" t="s">
-        <v>171</v>
+        <v>162</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="I5" t="s">
-        <v>256</v>
+        <v>166</v>
       </c>
       <c r="J5"/>
     </row>
@@ -3026,22 +3017,22 @@
         <v>47</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E6">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H6" s="45" t="s">
-        <v>173</v>
+        <v>157</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="I6" t="s">
-        <v>257</v>
+        <v>169</v>
       </c>
       <c r="J6"/>
     </row>
@@ -3052,22 +3043,22 @@
         <v>47</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E7">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H7" s="45" t="s">
-        <v>174</v>
+        <v>157</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="I7" t="s">
-        <v>258</v>
+        <v>171</v>
       </c>
       <c r="J7"/>
     </row>
@@ -3078,22 +3069,22 @@
         <v>47</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E8">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H8" s="45" t="s">
-        <v>175</v>
-      </c>
       <c r="I8" t="s">
-        <v>259</v>
+        <v>173</v>
       </c>
       <c r="J8"/>
     </row>
@@ -3104,22 +3095,22 @@
         <v>47</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E9">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H9" s="45" t="s">
-        <v>176</v>
+        <v>162</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="I9" t="s">
-        <v>260</v>
+        <v>175</v>
       </c>
       <c r="J9"/>
     </row>
@@ -3130,22 +3121,22 @@
         <v>47</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H10" s="45" t="s">
+      <c r="I10" t="s">
         <v>178</v>
-      </c>
-      <c r="I10" t="s">
-        <v>261</v>
       </c>
       <c r="J10"/>
     </row>
@@ -3156,22 +3147,22 @@
         <v>47</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H11" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>179</v>
       </c>
       <c r="I11" t="s">
-        <v>262</v>
+        <v>180</v>
       </c>
       <c r="J11"/>
     </row>
@@ -3182,22 +3173,22 @@
         <v>47</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H12" s="45" t="s">
-        <v>180</v>
+        <v>162</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="I12" t="s">
-        <v>263</v>
+        <v>182</v>
       </c>
       <c r="J12"/>
     </row>
@@ -3208,22 +3199,22 @@
         <v>47</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H13" s="45" t="s">
-        <v>181</v>
+        <v>162</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="I13" t="s">
-        <v>264</v>
+        <v>184</v>
       </c>
       <c r="J13"/>
     </row>
@@ -3234,22 +3225,22 @@
         <v>47</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E14">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H14" s="45" t="s">
-        <v>183</v>
+        <v>157</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="I14" t="s">
-        <v>265</v>
+        <v>187</v>
       </c>
       <c r="J14"/>
     </row>
@@ -3260,22 +3251,22 @@
         <v>47</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E15">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H15" s="45" t="s">
-        <v>184</v>
+        <v>157</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="I15" t="s">
-        <v>266</v>
+        <v>189</v>
       </c>
       <c r="J15"/>
     </row>
@@ -3286,22 +3277,22 @@
         <v>47</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E16">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H16" s="45" t="s">
-        <v>185</v>
+        <v>162</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="I16" t="s">
-        <v>267</v>
+        <v>191</v>
       </c>
       <c r="J16"/>
     </row>
@@ -3312,22 +3303,22 @@
         <v>47</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E17">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H17" s="45" t="s">
-        <v>186</v>
+        <v>162</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="I17" t="s">
-        <v>268</v>
+        <v>193</v>
       </c>
       <c r="J17"/>
     </row>
@@ -3338,22 +3329,22 @@
         <v>47</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E18">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H18" s="45" t="s">
-        <v>188</v>
+        <v>157</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="I18" t="s">
-        <v>269</v>
+        <v>196</v>
       </c>
       <c r="J18"/>
     </row>
@@ -3364,22 +3355,22 @@
         <v>47</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E19">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H19" s="45" t="s">
-        <v>189</v>
+        <v>157</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="I19" t="s">
-        <v>270</v>
+        <v>198</v>
       </c>
       <c r="J19"/>
     </row>
@@ -3390,22 +3381,22 @@
         <v>47</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E20">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H20" s="45" t="s">
-        <v>190</v>
+        <v>162</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="I20" t="s">
-        <v>271</v>
+        <v>200</v>
       </c>
       <c r="J20"/>
     </row>
@@ -3416,22 +3407,22 @@
         <v>47</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E21">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H21" s="45" t="s">
-        <v>191</v>
+        <v>162</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="I21" t="s">
-        <v>272</v>
+        <v>202</v>
       </c>
       <c r="J21"/>
     </row>
@@ -3442,22 +3433,22 @@
         <v>47</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E22">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H22" s="45" t="s">
-        <v>193</v>
+        <v>157</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="I22" t="s">
-        <v>273</v>
+        <v>205</v>
       </c>
       <c r="J22"/>
     </row>
@@ -3468,22 +3459,22 @@
         <v>47</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E23">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H23" s="45" t="s">
-        <v>194</v>
+        <v>157</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>206</v>
       </c>
       <c r="I23" t="s">
-        <v>274</v>
+        <v>207</v>
       </c>
       <c r="J23"/>
     </row>
@@ -3494,22 +3485,22 @@
         <v>47</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E24">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H24" s="45" t="s">
-        <v>195</v>
+        <v>162</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="I24" t="s">
-        <v>275</v>
+        <v>209</v>
       </c>
       <c r="J24"/>
     </row>
@@ -3520,22 +3511,22 @@
         <v>47</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E25">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H25" s="45" t="s">
-        <v>196</v>
+        <v>162</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="I25" t="s">
-        <v>276</v>
+        <v>211</v>
       </c>
       <c r="J25"/>
     </row>
@@ -3546,22 +3537,22 @@
         <v>47</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E26">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H26" s="45" t="s">
-        <v>198</v>
+        <v>157</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="I26" t="s">
-        <v>277</v>
+        <v>214</v>
       </c>
       <c r="J26"/>
     </row>
@@ -3572,22 +3563,22 @@
         <v>47</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E27">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H27" s="45" t="s">
-        <v>199</v>
+        <v>157</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="I27" t="s">
-        <v>278</v>
+        <v>216</v>
       </c>
       <c r="J27"/>
     </row>
@@ -3598,22 +3589,22 @@
         <v>47</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E28">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H28" s="45" t="s">
-        <v>200</v>
+        <v>162</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="I28" t="s">
-        <v>279</v>
+        <v>218</v>
       </c>
       <c r="J28"/>
     </row>
@@ -3624,22 +3615,22 @@
         <v>47</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E29">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H29" s="45" t="s">
-        <v>201</v>
+        <v>162</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>219</v>
       </c>
       <c r="I29" t="s">
-        <v>280</v>
+        <v>220</v>
       </c>
       <c r="J29"/>
     </row>
@@ -3650,22 +3641,22 @@
         <v>47</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>202</v>
+        <v>221</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H30" s="45" t="s">
-        <v>203</v>
+        <v>157</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="I30" t="s">
-        <v>281</v>
+        <v>223</v>
       </c>
       <c r="J30"/>
     </row>
@@ -3676,22 +3667,22 @@
         <v>47</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E31">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>202</v>
+        <v>221</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H31" s="45" t="s">
-        <v>204</v>
+        <v>157</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="I31" t="s">
-        <v>282</v>
+        <v>225</v>
       </c>
       <c r="J31"/>
     </row>
@@ -3702,22 +3693,22 @@
         <v>47</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E32">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>202</v>
+        <v>221</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H32" s="45" t="s">
-        <v>205</v>
+        <v>162</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="I32" t="s">
-        <v>283</v>
+        <v>227</v>
       </c>
       <c r="J32"/>
     </row>
@@ -3728,22 +3719,22 @@
         <v>47</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>202</v>
+        <v>221</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H33" s="45" t="s">
-        <v>206</v>
+        <v>162</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>228</v>
       </c>
       <c r="I33" t="s">
-        <v>284</v>
+        <v>229</v>
       </c>
       <c r="J33"/>
     </row>
@@ -3754,22 +3745,22 @@
         <v>47</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E34">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H34" s="45" t="s">
-        <v>208</v>
+        <v>157</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="I34" t="s">
-        <v>285</v>
+        <v>233</v>
       </c>
       <c r="J34"/>
     </row>
@@ -3780,22 +3771,22 @@
         <v>47</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E35">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H35" s="45" t="s">
-        <v>209</v>
+        <v>157</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="I35" t="s">
-        <v>286</v>
+        <v>235</v>
       </c>
       <c r="J35"/>
     </row>
@@ -3806,22 +3797,22 @@
         <v>47</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E36">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H36" s="45" t="s">
-        <v>210</v>
+        <v>162</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="I36" t="s">
-        <v>287</v>
+        <v>237</v>
       </c>
       <c r="J36"/>
     </row>
@@ -3832,22 +3823,22 @@
         <v>47</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E37">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H37" s="45" t="s">
-        <v>211</v>
+        <v>162</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="I37" t="s">
-        <v>288</v>
+        <v>239</v>
       </c>
       <c r="J37"/>
     </row>
@@ -3858,22 +3849,22 @@
         <v>47</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E38">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>212</v>
+        <v>240</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H38" s="45" t="s">
-        <v>213</v>
+        <v>157</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="I38" t="s">
-        <v>289</v>
+        <v>242</v>
       </c>
       <c r="J38"/>
     </row>
@@ -3884,22 +3875,22 @@
         <v>47</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E39">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>212</v>
+        <v>240</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H39" s="45" t="s">
-        <v>214</v>
+        <v>157</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>243</v>
       </c>
       <c r="I39" t="s">
-        <v>290</v>
+        <v>244</v>
       </c>
       <c r="J39"/>
     </row>
@@ -3910,22 +3901,22 @@
         <v>47</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E40">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>212</v>
+        <v>240</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H40" s="45" t="s">
-        <v>215</v>
+        <v>162</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>245</v>
       </c>
       <c r="I40" t="s">
-        <v>291</v>
+        <v>246</v>
       </c>
       <c r="J40"/>
     </row>
@@ -3936,22 +3927,22 @@
         <v>47</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E41">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>212</v>
+        <v>240</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H41" s="45" t="s">
-        <v>216</v>
+        <v>162</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>247</v>
       </c>
       <c r="I41" t="s">
-        <v>292</v>
+        <v>248</v>
       </c>
       <c r="J41"/>
     </row>
@@ -3962,22 +3953,22 @@
         <v>47</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E42">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>217</v>
+        <v>249</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H42" s="45" t="s">
-        <v>218</v>
+        <v>157</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="I42" t="s">
-        <v>293</v>
+        <v>251</v>
       </c>
       <c r="J42"/>
     </row>
@@ -3988,22 +3979,22 @@
         <v>47</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E43">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>217</v>
+        <v>249</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H43" s="45" t="s">
-        <v>219</v>
+        <v>157</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="I43" t="s">
-        <v>294</v>
+        <v>253</v>
       </c>
       <c r="J43"/>
     </row>
@@ -4014,22 +4005,22 @@
         <v>47</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E44">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>217</v>
+        <v>249</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H44" s="45" t="s">
-        <v>220</v>
+        <v>162</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>254</v>
       </c>
       <c r="I44" t="s">
-        <v>295</v>
+        <v>255</v>
       </c>
       <c r="J44"/>
     </row>
@@ -4040,22 +4031,22 @@
         <v>47</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E45">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>217</v>
+        <v>249</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H45" s="45" t="s">
-        <v>221</v>
+        <v>162</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>256</v>
       </c>
       <c r="I45" t="s">
-        <v>296</v>
+        <v>257</v>
       </c>
       <c r="J45"/>
     </row>
@@ -4066,22 +4057,22 @@
         <v>47</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E46">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H46" s="45" t="s">
-        <v>223</v>
+        <v>157</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>259</v>
       </c>
       <c r="I46" t="s">
-        <v>297</v>
+        <v>260</v>
       </c>
       <c r="J46"/>
     </row>
@@ -4092,460 +4083,460 @@
         <v>47</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E47">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H47" s="45" t="s">
-        <v>224</v>
+        <v>157</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="I47" t="s">
-        <v>298</v>
+        <v>262</v>
       </c>
       <c r="J47"/>
     </row>
-    <row r="48" spans="1:10" ht="30">
+    <row r="48" spans="1:10">
       <c r="A48" s="11"/>
       <c r="B48" s="11"/>
       <c r="C48" s="1">
         <v>47</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E48">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H48" s="45" t="s">
-        <v>225</v>
+        <v>162</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>263</v>
       </c>
       <c r="I48" t="s">
-        <v>299</v>
+        <v>264</v>
       </c>
       <c r="J48"/>
     </row>
-    <row r="49" spans="1:10" ht="30">
+    <row r="49" spans="1:10">
       <c r="A49" s="11"/>
       <c r="B49" s="11"/>
       <c r="C49" s="1">
         <v>47</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E49">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H49" s="45" t="s">
-        <v>226</v>
+        <v>162</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>265</v>
       </c>
       <c r="I49" t="s">
-        <v>300</v>
+        <v>266</v>
       </c>
       <c r="J49"/>
     </row>
-    <row r="50" spans="1:10" ht="30">
+    <row r="50" spans="1:10">
       <c r="A50" s="11"/>
       <c r="B50" s="11"/>
       <c r="C50" s="1">
         <v>47</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E50">
+        <v>14</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="I50" t="s">
+        <v>269</v>
+      </c>
+      <c r="J50"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="C51" s="1">
+        <v>47</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E51">
+        <v>14</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="I51" t="s">
+        <v>271</v>
+      </c>
+      <c r="J51"/>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="C52" s="1">
+        <v>47</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E52">
+        <v>14</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="I52" t="s">
+        <v>273</v>
+      </c>
+      <c r="J52"/>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="C53" s="1">
+        <v>47</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E53">
+        <v>14</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="I53" t="s">
+        <v>275</v>
+      </c>
+      <c r="J53"/>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="C54" s="1">
+        <v>47</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E54">
+        <v>16</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="I54" t="s">
+        <v>278</v>
+      </c>
+      <c r="J54"/>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="C55" s="1">
+        <v>47</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E55">
+        <v>16</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="I55" t="s">
+        <v>280</v>
+      </c>
+      <c r="J55"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="C56" s="1">
+        <v>47</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E56">
+        <v>16</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="I56" t="s">
+        <v>282</v>
+      </c>
+      <c r="J56"/>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="C57" s="1">
+        <v>47</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E57">
+        <v>16</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="I57" t="s">
+        <v>284</v>
+      </c>
+      <c r="J57"/>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="C58" s="1">
+        <v>47</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E58">
+        <v>8</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I58" t="s">
+        <v>287</v>
+      </c>
+      <c r="J58"/>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="C59" s="1">
+        <v>47</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E59">
+        <v>8</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I59" t="s">
+        <v>289</v>
+      </c>
+      <c r="J59"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="C60" s="1">
+        <v>47</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E60">
+        <v>8</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="I60" t="s">
+        <v>291</v>
+      </c>
+      <c r="J60"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="C61" s="1">
+        <v>47</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E61">
+        <v>8</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="I61" t="s">
+        <v>293</v>
+      </c>
+      <c r="J61"/>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="C62" s="1">
+        <v>47</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E62">
         <v>5</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H50" s="45" t="s">
-        <v>228</v>
-      </c>
-      <c r="I50" t="s">
+      <c r="F62" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="I62" t="s">
+        <v>296</v>
+      </c>
+      <c r="J62"/>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="C63" s="1">
+        <v>47</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E63">
+        <v>5</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I63" t="s">
+        <v>298</v>
+      </c>
+      <c r="J63"/>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="C64" s="1">
+        <v>47</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E64">
+        <v>5</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="I64" t="s">
+        <v>300</v>
+      </c>
+      <c r="J64"/>
+    </row>
+    <row r="65" spans="3:10">
+      <c r="C65" s="1">
+        <v>47</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E65">
+        <v>5</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H65" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="J50"/>
-    </row>
-    <row r="51" spans="1:10" ht="30">
-      <c r="C51" s="1">
-        <v>47</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E51">
-        <v>5</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H51" s="45" t="s">
-        <v>229</v>
-      </c>
-      <c r="I51" t="s">
+      <c r="I65" t="s">
         <v>302</v>
-      </c>
-      <c r="J51"/>
-    </row>
-    <row r="52" spans="1:10" ht="30">
-      <c r="C52" s="1">
-        <v>47</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E52">
-        <v>5</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H52" s="45" t="s">
-        <v>230</v>
-      </c>
-      <c r="I52" t="s">
-        <v>303</v>
-      </c>
-      <c r="J52"/>
-    </row>
-    <row r="53" spans="1:10" ht="30">
-      <c r="C53" s="1">
-        <v>47</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E53">
-        <v>5</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H53" s="45" t="s">
-        <v>231</v>
-      </c>
-      <c r="I53" t="s">
-        <v>304</v>
-      </c>
-      <c r="J53"/>
-    </row>
-    <row r="54" spans="1:10" ht="30">
-      <c r="C54" s="1">
-        <v>47</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E54">
-        <v>3</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H54" s="45" t="s">
-        <v>233</v>
-      </c>
-      <c r="I54" t="s">
-        <v>305</v>
-      </c>
-      <c r="J54"/>
-    </row>
-    <row r="55" spans="1:10" ht="30">
-      <c r="C55" s="1">
-        <v>47</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E55">
-        <v>3</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H55" s="45" t="s">
-        <v>234</v>
-      </c>
-      <c r="I55" t="s">
-        <v>306</v>
-      </c>
-      <c r="J55"/>
-    </row>
-    <row r="56" spans="1:10" ht="30">
-      <c r="C56" s="1">
-        <v>47</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E56">
-        <v>3</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H56" s="45" t="s">
-        <v>235</v>
-      </c>
-      <c r="I56" t="s">
-        <v>307</v>
-      </c>
-      <c r="J56"/>
-    </row>
-    <row r="57" spans="1:10" ht="30">
-      <c r="C57" s="1">
-        <v>47</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E57">
-        <v>3</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H57" s="45" t="s">
-        <v>236</v>
-      </c>
-      <c r="I57" t="s">
-        <v>308</v>
-      </c>
-      <c r="J57"/>
-    </row>
-    <row r="58" spans="1:10" ht="30">
-      <c r="C58" s="1">
-        <v>47</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E58">
-        <v>10</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H58" s="45" t="s">
-        <v>238</v>
-      </c>
-      <c r="I58" t="s">
-        <v>309</v>
-      </c>
-      <c r="J58"/>
-    </row>
-    <row r="59" spans="1:10" ht="30">
-      <c r="C59" s="1">
-        <v>47</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E59">
-        <v>10</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H59" s="45" t="s">
-        <v>239</v>
-      </c>
-      <c r="I59" t="s">
-        <v>310</v>
-      </c>
-      <c r="J59"/>
-    </row>
-    <row r="60" spans="1:10" ht="30">
-      <c r="C60" s="1">
-        <v>47</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E60">
-        <v>10</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H60" s="45" t="s">
-        <v>240</v>
-      </c>
-      <c r="I60" t="s">
-        <v>311</v>
-      </c>
-      <c r="J60"/>
-    </row>
-    <row r="61" spans="1:10" ht="30">
-      <c r="C61" s="1">
-        <v>47</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E61">
-        <v>10</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H61" s="45" t="s">
-        <v>241</v>
-      </c>
-      <c r="I61" t="s">
-        <v>312</v>
-      </c>
-      <c r="J61"/>
-    </row>
-    <row r="62" spans="1:10" ht="30">
-      <c r="C62" s="1">
-        <v>47</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E62">
-        <v>9</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H62" s="45" t="s">
-        <v>243</v>
-      </c>
-      <c r="I62" t="s">
-        <v>313</v>
-      </c>
-      <c r="J62"/>
-    </row>
-    <row r="63" spans="1:10" ht="30">
-      <c r="C63" s="1">
-        <v>47</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E63">
-        <v>9</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H63" s="45" t="s">
-        <v>244</v>
-      </c>
-      <c r="I63" t="s">
-        <v>314</v>
-      </c>
-      <c r="J63"/>
-    </row>
-    <row r="64" spans="1:10" ht="30">
-      <c r="C64" s="1">
-        <v>47</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E64">
-        <v>9</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H64" s="45" t="s">
-        <v>245</v>
-      </c>
-      <c r="I64" t="s">
-        <v>315</v>
-      </c>
-      <c r="J64"/>
-    </row>
-    <row r="65" spans="3:10" ht="30">
-      <c r="C65" s="1">
-        <v>47</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E65">
-        <v>9</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H65" s="45" t="s">
-        <v>246</v>
-      </c>
-      <c r="I65" t="s">
-        <v>316</v>
       </c>
       <c r="J65"/>
     </row>
@@ -4579,7 +4570,7 @@
   <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4654,10 +4645,10 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>247</v>
+        <v>148</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K2">
         <f>I2*1000</f>
@@ -4683,10 +4674,10 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>248</v>
+        <v>150</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K3"/>
       <c r="L3"/>
@@ -4703,10 +4694,10 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>249</v>
+        <v>151</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K4"/>
       <c r="L4"/>
@@ -4723,10 +4714,10 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>250</v>
+        <v>152</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K5"/>
       <c r="L5"/>
@@ -4743,10 +4734,10 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>251</v>
+        <v>153</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K6"/>
       <c r="L6"/>
@@ -4763,10 +4754,10 @@
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>252</v>
+        <v>154</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K7"/>
       <c r="L7"/>
@@ -5282,8 +5273,8 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="50.1" customHeight="1"/>

</xml_diff>